<commit_message>
WIP V13 with numerical arguments
</commit_message>
<xml_diff>
--- a/src/lithium/data/La Compil pour Yann.xlsx
+++ b/src/lithium/data/La Compil pour Yann.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="8220" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>Li+ext (mM)</t>
   </si>
   <si>
-    <t>Dose réponse à 37°C</t>
-  </si>
-  <si>
     <t>Cinétique de NHE1 temps courts. 37°C-15mM Lithium extracellulaire.</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t xml:space="preserve"> NHE1</t>
+  </si>
+  <si>
+    <t>Dose réponse à 37°C, 1 minute</t>
   </si>
 </sst>
 </file>
@@ -836,7 +836,7 @@
             <c:numRef>
               <c:f>Feuil1!$E$31:$E$37</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>57.48417141584081</c:v>
@@ -872,11 +872,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2020028072"/>
-        <c:axId val="2020040120"/>
+        <c:axId val="2063375240"/>
+        <c:axId val="2063375768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2020028072"/>
+        <c:axId val="2063375240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,13 +886,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2020040120"/>
+        <c:crossAx val="2063375768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2020040120"/>
+        <c:axId val="2063375768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1800.0"/>
@@ -907,11 +907,11 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2020028072"/>
+        <c:crossAx val="2063375240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500.0"/>
@@ -1042,11 +1042,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2020426056"/>
-        <c:axId val="2019880104"/>
+        <c:axId val="2063409864"/>
+        <c:axId val="2063412728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2020426056"/>
+        <c:axId val="2063409864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,12 +1056,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2019880104"/>
+        <c:crossAx val="2063412728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2019880104"/>
+        <c:axId val="2063412728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2020426056"/>
+        <c:crossAx val="2063409864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1151,7 +1151,7 @@
             <c:numRef>
               <c:f>Feuil1!$E$5:$E$9</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>64.8414985590778</c:v>
@@ -1181,11 +1181,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2141860120"/>
-        <c:axId val="-2141638136"/>
+        <c:axId val="2082395016"/>
+        <c:axId val="2082398040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2141860120"/>
+        <c:axId val="2082395016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,23 +1195,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141638136"/>
+        <c:crossAx val="2082398040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2141638136"/>
+        <c:axId val="2082398040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141860120"/>
+        <c:crossAx val="2082395016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1293,7 +1293,7 @@
             <c:numRef>
               <c:f>Feuil1!$F$14:$F$21</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0,000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1.3154069</c:v>
@@ -1332,11 +1332,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2042437896"/>
-        <c:axId val="-2141901480"/>
+        <c:axId val="2082421576"/>
+        <c:axId val="2082424664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2042437896"/>
+        <c:axId val="2082421576"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1347,23 +1347,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141901480"/>
+        <c:crossAx val="2082424664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2141901480"/>
+        <c:axId val="2082424664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="0,000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2042437896"/>
+        <c:crossAx val="2082421576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1442,7 +1442,7 @@
             <c:numRef>
               <c:f>Feuil1!$C$43:$C$49</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0,000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>5.37</c:v>
@@ -1478,11 +1478,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2041833976"/>
-        <c:axId val="2041837064"/>
+        <c:axId val="2082448520"/>
+        <c:axId val="2082451608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2041833976"/>
+        <c:axId val="2082448520"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1493,23 +1493,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2041837064"/>
+        <c:crossAx val="2082451608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2041837064"/>
+        <c:axId val="2082451608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="0,000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2041833976"/>
+        <c:crossAx val="2082448520"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1618,11 +1618,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2041808728"/>
-        <c:axId val="2041796504"/>
+        <c:axId val="2081830024"/>
+        <c:axId val="2081827032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2041808728"/>
+        <c:axId val="2081830024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1641,7 +1641,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2041796504"/>
+        <c:crossAx val="2081827032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1649,7 +1649,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2041796504"/>
+        <c:axId val="2081827032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1676,7 +1676,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2041808728"/>
+        <c:crossAx val="2081830024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2.0"/>
@@ -2206,8 +2206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130:C130"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2221,7 +2221,7 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="7"/>
     </row>
@@ -2252,14 +2252,14 @@
     <row r="4" spans="1:15">
       <c r="A4" s="1"/>
       <c r="B4" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -2417,13 +2417,13 @@
         <v>2017</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="31"/>
     </row>
     <row r="13" spans="1:15">
       <c r="B13" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>0</v>
@@ -2435,7 +2435,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -2567,7 +2567,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="B23" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2578,19 +2578,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="7" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="B29" s="9"/>
       <c r="C29" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>6</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2598,19 +2598,19 @@
         <v>3</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2768,7 +2768,7 @@
     </row>
     <row r="38" spans="2:16">
       <c r="G38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:16">
@@ -2903,38 +2903,38 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="16">
       <c r="B58" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="C58" s="57" t="s">
+      <c r="D58" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" s="57" t="s">
+      <c r="F58" s="57" t="s">
         <v>61</v>
-      </c>
-      <c r="F58" s="57" t="s">
-        <v>62</v>
       </c>
       <c r="G58" s="57" t="s">
         <v>0</v>
       </c>
       <c r="H58" s="57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B59" s="53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C59" s="53">
         <v>37</v>
@@ -2953,7 +2953,7 @@
     </row>
     <row r="60" spans="1:10">
       <c r="B60" s="54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C60" s="55">
         <v>37</v>
@@ -2976,7 +2976,7 @@
     </row>
     <row r="61" spans="1:10">
       <c r="B61" s="54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C61" s="55">
         <v>37</v>
@@ -2999,7 +2999,7 @@
     </row>
     <row r="62" spans="1:10">
       <c r="B62" s="54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C62" s="55">
         <v>37</v>
@@ -3022,7 +3022,7 @@
     </row>
     <row r="63" spans="1:10">
       <c r="B63" s="54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C63" s="55">
         <v>21</v>
@@ -3047,7 +3047,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3055,7 +3055,7 @@
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3063,13 +3063,13 @@
     </row>
     <row r="71" spans="1:5">
       <c r="B71" s="38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C71" s="31"/>
     </row>
     <row r="72" spans="1:5">
       <c r="B72" s="39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C72" s="40">
         <v>11.472061</v>
@@ -3077,7 +3077,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="B73" s="39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C73" s="40">
         <v>8.2891432999999992</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="B74" s="39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C74" s="40">
         <f>AVERAGE(D74:E74)</f>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="75" spans="1:5">
       <c r="B75" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C75" s="41">
         <f>AVERAGE(C72:C74)</f>
@@ -3109,14 +3109,14 @@
     </row>
     <row r="78" spans="1:5">
       <c r="B78" s="42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C78" s="43"/>
       <c r="D78" s="43"/>
     </row>
     <row r="79" spans="1:5">
       <c r="B79" s="43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C79" s="43">
         <v>13.76</v>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="80" spans="1:5">
       <c r="B80" s="43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C80">
         <f>AVERAGE(D80:E80)</f>
@@ -3140,7 +3140,7 @@
     </row>
     <row r="81" spans="2:7">
       <c r="B81" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(C79:C80)</f>
@@ -3149,17 +3149,17 @@
     </row>
     <row r="83" spans="2:7">
       <c r="B83" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="84" spans="2:7">
       <c r="B84" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="85" spans="2:7">
       <c r="B85" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C85">
         <v>4.53</v>
@@ -3167,7 +3167,7 @@
     </row>
     <row r="86" spans="2:7">
       <c r="B86" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C86">
         <v>3.16</v>
@@ -3175,10 +3175,10 @@
     </row>
     <row r="87" spans="2:7">
       <c r="E87" s="50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F87" s="50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G87" s="50">
         <v>1.24</v>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="89" spans="2:7">
       <c r="B89" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C89">
         <v>6.5798797999999996</v>
@@ -3194,7 +3194,7 @@
     </row>
     <row r="90" spans="2:7">
       <c r="B90" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C90">
         <v>5.1079268999999998</v>
@@ -3202,7 +3202,7 @@
     </row>
     <row r="91" spans="2:7">
       <c r="B91" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C91">
         <v>6.4017175000000002</v>
@@ -3210,7 +3210,7 @@
     </row>
     <row r="92" spans="2:7">
       <c r="B92" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C92">
         <v>3.9291575999999999</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="93" spans="2:7">
       <c r="B93" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(C89:C92)</f>
@@ -3227,7 +3227,7 @@
     </row>
     <row r="96" spans="2:7">
       <c r="B96" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(C79:C92)</f>
@@ -3236,12 +3236,12 @@
     </row>
     <row r="99" spans="2:3">
       <c r="B99" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="2:3">
       <c r="B100" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C100">
         <v>6.46</v>
@@ -3249,7 +3249,7 @@
     </row>
     <row r="101" spans="2:3">
       <c r="B101" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C101">
         <v>3.52</v>
@@ -3257,12 +3257,12 @@
     </row>
     <row r="102" spans="2:3">
       <c r="B102" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="103" spans="2:3">
       <c r="B103" s="44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C103" s="44">
         <v>5.98</v>
@@ -3270,7 +3270,7 @@
     </row>
     <row r="104" spans="2:3">
       <c r="B104" s="51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(C100:C103)</f>
@@ -3279,12 +3279,12 @@
     </row>
     <row r="106" spans="2:3">
       <c r="B106" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="108" spans="2:3">
       <c r="B108" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C108">
         <v>13.27</v>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="109" spans="2:3">
       <c r="B109" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C109">
         <v>16.649999999999999</v>
@@ -3300,7 +3300,7 @@
     </row>
     <row r="110" spans="2:3">
       <c r="B110" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(C108:C109)</f>
@@ -3309,7 +3309,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="B113" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(C72:C109)</f>
@@ -3318,7 +3318,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C117" t="s">
         <v>0</v>
@@ -3326,7 +3326,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="B119" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C119" s="45">
         <v>13.8</v>
@@ -3334,7 +3334,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="B120" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C120" s="45">
         <v>13.6</v>
@@ -3377,7 +3377,7 @@
     </row>
     <row r="130" spans="2:3">
       <c r="B130" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C130" s="52">
         <f>AVERAGE(C119:C126)</f>

</xml_diff>

<commit_message>
need to express dose-response concentration
</commit_message>
<xml_diff>
--- a/src/lithium/data/La Compil pour Yann.xlsx
+++ b/src/lithium/data/La Compil pour Yann.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37620" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -419,8 +419,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -632,7 +646,7 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="133">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -692,6 +706,13 @@
     <cellStyle name="Lien hypertexte" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -751,6 +772,13 @@
     <cellStyle name="Lien hypertexte visité" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -872,11 +900,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2063375240"/>
-        <c:axId val="2063375768"/>
+        <c:axId val="-2127064744"/>
+        <c:axId val="-2127063656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2063375240"/>
+        <c:axId val="-2127064744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,13 +914,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063375768"/>
+        <c:crossAx val="-2127063656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2063375768"/>
+        <c:axId val="-2127063656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1800.0"/>
@@ -911,7 +939,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063375240"/>
+        <c:crossAx val="-2127064744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500.0"/>
@@ -1042,11 +1070,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2063409864"/>
-        <c:axId val="2063412728"/>
+        <c:axId val="2033569256"/>
+        <c:axId val="2033566392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2063409864"/>
+        <c:axId val="2033569256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,12 +1084,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063412728"/>
+        <c:crossAx val="2033566392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2063412728"/>
+        <c:axId val="2033566392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1106,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063409864"/>
+        <c:crossAx val="2033569256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1181,11 +1209,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2082395016"/>
-        <c:axId val="2082398040"/>
+        <c:axId val="2033543304"/>
+        <c:axId val="2033540280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2082395016"/>
+        <c:axId val="2033543304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,12 +1223,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082398040"/>
+        <c:crossAx val="2033540280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2082398040"/>
+        <c:axId val="2033540280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1211,7 +1239,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082395016"/>
+        <c:crossAx val="2033543304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1332,11 +1360,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2082421576"/>
-        <c:axId val="2082424664"/>
+        <c:axId val="2033516728"/>
+        <c:axId val="2033513640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2082421576"/>
+        <c:axId val="2033516728"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1347,12 +1375,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082424664"/>
+        <c:crossAx val="2033513640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2082424664"/>
+        <c:axId val="2033513640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1363,7 +1391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082421576"/>
+        <c:crossAx val="2033516728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1478,11 +1506,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2082448520"/>
-        <c:axId val="2082451608"/>
+        <c:axId val="2033490024"/>
+        <c:axId val="2033486936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2082448520"/>
+        <c:axId val="2033490024"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1493,12 +1521,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082451608"/>
+        <c:crossAx val="2033486936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2082451608"/>
+        <c:axId val="2033486936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,7 +1537,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082448520"/>
+        <c:crossAx val="2033490024"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1618,11 +1646,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2081830024"/>
-        <c:axId val="2081827032"/>
+        <c:axId val="-2128874312"/>
+        <c:axId val="-2128871288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2081830024"/>
+        <c:axId val="-2128874312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1641,7 +1669,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081827032"/>
+        <c:crossAx val="-2128871288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1649,7 +1677,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081827032"/>
+        <c:axId val="-2128871288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1676,7 +1704,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081830024"/>
+        <c:crossAx val="-2128874312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2.0"/>
@@ -2206,8 +2234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>